<commit_message>
Update Sensor Bits per Second Optimizing.xlsx
</commit_message>
<xml_diff>
--- a/4 Sensors/Sensor Bits per Second Optimizing.xlsx
+++ b/4 Sensors/Sensor Bits per Second Optimizing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\OneDrive\Documents\GitHub\GTOR-DAQ\4 Sensors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED274241-FD23-49A1-8488-08CCBDFA942B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A225CF87-A6A4-4C0C-AD49-AC7E42CF5EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{2C266F95-D56F-4A56-B616-ACDAB9F5864D}"/>
   </bookViews>
@@ -206,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -217,10 +217,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,7 +926,7 @@
         <v>50</v>
       </c>
       <c r="G3" s="2">
-        <f>D3*E3*F3</f>
+        <f t="shared" ref="G3:G14" si="0">D3*E3*F3</f>
         <v>800</v>
       </c>
     </row>
@@ -948,7 +947,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="2">
-        <f>D4*E4*F4</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -969,7 +968,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="2">
-        <f>D5*E5*F5</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -990,7 +989,7 @@
         <v>50</v>
       </c>
       <c r="G6" s="2">
-        <f>D6*E6*F6</f>
+        <f t="shared" si="0"/>
         <v>4800</v>
       </c>
     </row>
@@ -1011,7 +1010,7 @@
         <v>2</v>
       </c>
       <c r="G7" s="2">
-        <f>D7*E7*F7</f>
+        <f t="shared" si="0"/>
         <v>192</v>
       </c>
     </row>
@@ -1032,7 +1031,7 @@
         <v>40</v>
       </c>
       <c r="G8" s="2">
-        <f>D8*E8*F8</f>
+        <f t="shared" si="0"/>
         <v>960</v>
       </c>
     </row>
@@ -1053,7 +1052,7 @@
         <v>40</v>
       </c>
       <c r="G9" s="2">
-        <f>D9*E9*F9</f>
+        <f t="shared" si="0"/>
         <v>1280</v>
       </c>
     </row>
@@ -1074,7 +1073,7 @@
         <v>10</v>
       </c>
       <c r="G10" s="2">
-        <f>D10*E10*F10</f>
+        <f t="shared" si="0"/>
         <v>960</v>
       </c>
     </row>
@@ -1095,7 +1094,7 @@
         <v>2</v>
       </c>
       <c r="G11" s="2">
-        <f>D11*E11*F11</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
@@ -1116,7 +1115,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="2">
-        <f>D12*E12*F12</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
     </row>
@@ -1137,7 +1136,7 @@
         <v>2</v>
       </c>
       <c r="G13" s="2">
-        <f>D13*E13*F13</f>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
@@ -1158,7 +1157,7 @@
         <v>40</v>
       </c>
       <c r="G14" s="2">
-        <f>D14*E14*F14</f>
+        <f t="shared" si="0"/>
         <v>480</v>
       </c>
     </row>
@@ -1170,11 +1169,11 @@
         <v>17</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" ref="D15:E15" si="0">SUM(D3:D14)</f>
+        <f t="shared" ref="D15:E15" si="1">SUM(D3:D14)</f>
         <v>21</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>206</v>
       </c>
       <c r="F15" s="3">
@@ -1199,330 +1198,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF8327AF-D7B5-451E-AAAC-66108A1AFCA9}">
-  <dimension ref="B1:G18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="5" width="22" customWidth="1"/>
-    <col min="6" max="7" width="21.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2">
-        <v>50</v>
-      </c>
-      <c r="G3" s="2">
-        <f>D3*E3*F3</f>
-        <v>800</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2">
-        <v>10</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" ref="G4:G14" si="0">D4*E4*F4</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="2">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="2">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="2">
-        <v>3</v>
-      </c>
-      <c r="E6" s="2">
-        <v>32</v>
-      </c>
-      <c r="F6" s="2">
-        <v>50</v>
-      </c>
-      <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>4800</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="2">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="2">
-        <v>3</v>
-      </c>
-      <c r="E7" s="2">
-        <v>32</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>96</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="2">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="2">
-        <v>2</v>
-      </c>
-      <c r="E8" s="2">
-        <v>12</v>
-      </c>
-      <c r="F8" s="2">
-        <v>20</v>
-      </c>
-      <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>480</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="2">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1</v>
-      </c>
-      <c r="E9" s="2">
-        <v>32</v>
-      </c>
-      <c r="F9" s="2">
-        <v>20</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>640</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="2">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="2">
-        <v>3</v>
-      </c>
-      <c r="E10" s="2">
-        <v>32</v>
-      </c>
-      <c r="F10" s="2">
-        <v>5</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>480</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="2">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2">
-        <v>12</v>
-      </c>
-      <c r="F11" s="2">
-        <v>1</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="2">
-        <v>10</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2">
-        <v>1</v>
-      </c>
-      <c r="E12" s="2">
-        <v>12</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="2">
-        <v>11</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2">
-        <v>3</v>
-      </c>
-      <c r="E13" s="2">
-        <v>12</v>
-      </c>
-      <c r="F13" s="2">
-        <v>1</v>
-      </c>
-      <c r="G13" s="2">
-        <f>D13*E13*F13</f>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="2">
-        <v>12</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2">
-        <v>12</v>
-      </c>
-      <c r="F14" s="2">
-        <v>20</v>
-      </c>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>240</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="3">
-        <f t="shared" ref="D15:F15" si="1">SUM(D3:D14)</f>
-        <v>21</v>
-      </c>
-      <c r="E15" s="3">
-        <f t="shared" si="1"/>
-        <v>206</v>
-      </c>
-      <c r="F15" s="3">
-        <f t="shared" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="G15" s="3">
-        <f>SUM(G3:G14)</f>
-        <v>7607</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="C17" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C18" s="5"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0B2FC7C-1C3F-4B04-A5F6-CE4CF730119C}">
   <dimension ref="B1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1570,6 +1245,327 @@
         <v>16</v>
       </c>
       <c r="F3" s="2">
+        <v>50</v>
+      </c>
+      <c r="G3" s="2">
+        <f>D3*E3*F3</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" ref="G4:G14" si="0">D4*E4*F4</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>32</v>
+      </c>
+      <c r="F6" s="2">
+        <v>50</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="0"/>
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2">
+        <v>32</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>12</v>
+      </c>
+      <c r="F8" s="2">
+        <v>20</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="2">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>32</v>
+      </c>
+      <c r="F9" s="2">
+        <v>20</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>32</v>
+      </c>
+      <c r="F10" s="2">
+        <v>5</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>12</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="2">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>12</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="2">
+        <v>11</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="2">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2">
+        <v>12</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <f>D13*E13*F13</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="2">
+        <v>12</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>12</v>
+      </c>
+      <c r="F14" s="2">
+        <v>20</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" ref="D15:F15" si="1">SUM(D3:D14)</f>
+        <v>21</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="1"/>
+        <v>206</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
+      <c r="G15" s="3">
+        <f>SUM(G3:G14)</f>
+        <v>7607</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="C17" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0B2FC7C-1C3F-4B04-A5F6-CE4CF730119C}">
+  <dimension ref="B1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="5" width="22" customWidth="1"/>
+    <col min="6" max="7" width="21.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2">
         <v>10</v>
       </c>
       <c r="G3" s="2">
@@ -1717,11 +1713,11 @@
         <v>32</v>
       </c>
       <c r="F10" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>192</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
@@ -1825,11 +1821,11 @@
       </c>
       <c r="F15" s="3">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G15" s="3">
         <f>SUM(G3:G14)</f>
-        <v>2042</v>
+        <v>2138</v>
       </c>
     </row>
     <row r="17" spans="3:3" ht="23.4" x14ac:dyDescent="0.3">
@@ -2810,11 +2806,12 @@
   <dimension ref="B1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="8.88671875" customWidth="1"/>
     <col min="2" max="5" width="22" customWidth="1"/>
     <col min="6" max="7" width="21.77734375" customWidth="1"/>
   </cols>

</xml_diff>